<commit_message>
Corrections to errors on FC calculations
</commit_message>
<xml_diff>
--- a/Examples/BarometryTests/Plag2Pyx/LowP.xlsx
+++ b/Examples/BarometryTests/Plag2Pyx/LowP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\2022\GitHub\pyMELTScalc\Examples\BarometryTests\Plag2Pyx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\2022\GitHub\pyMELTScalc\Examples\BarometryTests\Plag2Pyx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8558606-F5C0-41A0-8B89-8EF7D86E7C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F01A4C-71DD-47C8-A471-8DF557F21554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8A1BF5-5808-4F4E-8D9C-08A3480DCA11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3F8A1BF5-5808-4F4E-8D9C-08A3480DCA11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -688,13 +688,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344AA545-37EC-4022-88E4-EAB9C9DA4E76}">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E38" sqref="E37:P38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,7 +759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -818,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -880,7 +883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -942,7 +945,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>4.0019999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>4.0149999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>4.1470000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1376,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1562,7 +1565,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1810,7 +1813,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1872,7 +1875,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>2.0219999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>2.0219999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2058,7 +2061,7 @@
         <v>2.004</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2120,7 +2123,7 @@
         <v>2.0219999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>4.1349999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2244,7 +2247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2306,7 +2309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -2430,7 +2433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2554,7 +2557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -2678,7 +2681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
@@ -2739,7 +2742,7 @@
       </c>
       <c r="U33" s="7"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>67</v>
       </c>
@@ -2800,7 +2803,7 @@
       </c>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -2861,7 +2864,7 @@
       </c>
       <c r="U35" s="7"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>72</v>
       </c>
@@ -2922,7 +2925,7 @@
       </c>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>75</v>
       </c>
@@ -2983,7 +2986,7 @@
       </c>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>75</v>
       </c>
@@ -3044,7 +3047,7 @@
       </c>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>75</v>
       </c>

</xml_diff>